<commit_message>
Worked on Filter performance évaluation
</commit_message>
<xml_diff>
--- a/00_Documentation/rapport/eval_perf/Resultat.xlsx
+++ b/00_Documentation/rapport/eval_perf/Resultat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salyd\Repos\stm32pdm\00_Documentation\rapport\eval_perf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A392D77-06D9-4634-A250-19C5C327CED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D21E369-EC95-4578-AE5D-4976733F34D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8EC1BED5-1BA0-4C04-B356-8626654CD591}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8EC1BED5-1BA0-4C04-B356-8626654CD591}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Temps Buffer</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>HCLK</t>
+  </si>
+  <si>
+    <t>Temps Flag (µs)</t>
+  </si>
+  <si>
+    <t>Temps Filtrage (µs)</t>
   </si>
 </sst>
 </file>
@@ -470,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF5887B-EB15-4CD7-BB55-355FC697C349}">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,10 +517,10 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -591,7 +597,7 @@
         <v>64</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C27" si="0">B5*A5</f>
+        <f t="shared" ref="C5:C17" si="0">B5*A5</f>
         <v>1024000</v>
       </c>
       <c r="D5">
@@ -601,7 +607,7 @@
         <v>150</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ref="F5:F27" si="1">E5/D5</f>
+        <f t="shared" ref="F5:F17" si="1">E5/D5</f>
         <v>0.15</v>
       </c>
       <c r="G5" s="1">
@@ -624,7 +630,7 @@
         <v>25</v>
       </c>
       <c r="M5">
-        <f t="shared" ref="M5:M27" si="3">((1/I5)*J5/(K5*L5))/0.064</f>
+        <f t="shared" ref="M5:M17" si="3">((1/I5)*J5/(K5*L5))/0.064</f>
         <v>2</v>
       </c>
     </row>
@@ -1275,7 +1281,7 @@
         <v>64</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:C35" si="4">B23*A23</f>
+        <f t="shared" ref="C23:C45" si="4">B23*A23</f>
         <v>1024000</v>
       </c>
       <c r="D23">
@@ -1305,7 +1311,7 @@
         <v>25</v>
       </c>
       <c r="M23">
-        <f t="shared" ref="M23:M35" si="6">((1/I23)*J23/(K23*L23))/0.064</f>
+        <f t="shared" ref="M23:M45" si="6">((1/I23)*J23/(K23*L23))/0.064</f>
         <v>2</v>
       </c>
     </row>
@@ -1811,6 +1817,1475 @@
       <c r="M35">
         <f t="shared" si="6"/>
         <v>14.000000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>120000</v>
+      </c>
+      <c r="B36">
+        <v>64</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="4"/>
+        <v>7680000</v>
+      </c>
+      <c r="D36">
+        <v>1000</v>
+      </c>
+      <c r="E36">
+        <v>612</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" ref="F36:F45" si="7">E36/D36</f>
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" ref="G36:G45" si="8">1-F36</f>
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="I36">
+        <v>5</v>
+      </c>
+      <c r="J36">
+        <v>120</v>
+      </c>
+      <c r="K36">
+        <v>5</v>
+      </c>
+      <c r="L36">
+        <v>5</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>128000</v>
+      </c>
+      <c r="B37">
+        <v>64</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="4"/>
+        <v>8192000</v>
+      </c>
+      <c r="D37">
+        <v>1000</v>
+      </c>
+      <c r="E37">
+        <v>652</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="7"/>
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="G37" s="1">
+        <f t="shared" si="8"/>
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="I37">
+        <v>5</v>
+      </c>
+      <c r="J37">
+        <v>128</v>
+      </c>
+      <c r="K37">
+        <v>5</v>
+      </c>
+      <c r="L37">
+        <v>5</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>136000</v>
+      </c>
+      <c r="B38">
+        <v>64</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="4"/>
+        <v>8704000</v>
+      </c>
+      <c r="D38">
+        <v>1000</v>
+      </c>
+      <c r="E38">
+        <v>696</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="7"/>
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="8"/>
+        <v>0.30400000000000005</v>
+      </c>
+      <c r="I38">
+        <v>5</v>
+      </c>
+      <c r="J38">
+        <v>136</v>
+      </c>
+      <c r="K38">
+        <v>5</v>
+      </c>
+      <c r="L38">
+        <v>5</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>144000</v>
+      </c>
+      <c r="B39">
+        <v>64</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="4"/>
+        <v>9216000</v>
+      </c>
+      <c r="D39">
+        <v>1000</v>
+      </c>
+      <c r="E39">
+        <v>736</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="7"/>
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="G39" s="1">
+        <f t="shared" si="8"/>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="I39">
+        <v>5</v>
+      </c>
+      <c r="J39">
+        <v>144</v>
+      </c>
+      <c r="K39">
+        <v>5</v>
+      </c>
+      <c r="L39">
+        <v>5</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>152000</v>
+      </c>
+      <c r="B40">
+        <v>64</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="4"/>
+        <v>9728000</v>
+      </c>
+      <c r="D40">
+        <v>1000</v>
+      </c>
+      <c r="E40">
+        <v>776</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="7"/>
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" si="8"/>
+        <v>0.22399999999999998</v>
+      </c>
+      <c r="I40">
+        <v>5</v>
+      </c>
+      <c r="J40">
+        <v>152</v>
+      </c>
+      <c r="K40">
+        <v>5</v>
+      </c>
+      <c r="L40">
+        <v>5</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="6"/>
+        <v>19.000000000000004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>160000</v>
+      </c>
+      <c r="B41">
+        <v>64</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="4"/>
+        <v>10240000</v>
+      </c>
+      <c r="D41">
+        <v>1000</v>
+      </c>
+      <c r="E41">
+        <v>816</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="7"/>
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="8"/>
+        <v>0.18400000000000005</v>
+      </c>
+      <c r="I41">
+        <v>5</v>
+      </c>
+      <c r="J41">
+        <v>160</v>
+      </c>
+      <c r="K41">
+        <v>5</v>
+      </c>
+      <c r="L41">
+        <v>5</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>168000</v>
+      </c>
+      <c r="B42">
+        <v>64</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="4"/>
+        <v>10752000</v>
+      </c>
+      <c r="D42">
+        <v>1000</v>
+      </c>
+      <c r="E42">
+        <v>860</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="7"/>
+        <v>0.86</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="8"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I42">
+        <v>5</v>
+      </c>
+      <c r="J42">
+        <v>168</v>
+      </c>
+      <c r="K42">
+        <v>5</v>
+      </c>
+      <c r="L42">
+        <v>5</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>176000</v>
+      </c>
+      <c r="B43">
+        <v>64</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="4"/>
+        <v>11264000</v>
+      </c>
+      <c r="D43">
+        <v>1000</v>
+      </c>
+      <c r="E43">
+        <v>896</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="7"/>
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="8"/>
+        <v>0.10399999999999998</v>
+      </c>
+      <c r="I43">
+        <v>5</v>
+      </c>
+      <c r="J43">
+        <v>176</v>
+      </c>
+      <c r="K43">
+        <v>5</v>
+      </c>
+      <c r="L43">
+        <v>5</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>184000</v>
+      </c>
+      <c r="B44">
+        <v>64</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="4"/>
+        <v>11776000</v>
+      </c>
+      <c r="D44">
+        <v>1000</v>
+      </c>
+      <c r="E44">
+        <v>940</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="7"/>
+        <v>0.94</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="8"/>
+        <v>6.0000000000000053E-2</v>
+      </c>
+      <c r="I44">
+        <v>5</v>
+      </c>
+      <c r="J44">
+        <v>184</v>
+      </c>
+      <c r="K44">
+        <v>5</v>
+      </c>
+      <c r="L44">
+        <v>5</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="6"/>
+        <v>23.000000000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>192000</v>
+      </c>
+      <c r="B45">
+        <v>64</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="4"/>
+        <v>12288000</v>
+      </c>
+      <c r="D45">
+        <v>1000</v>
+      </c>
+      <c r="E45">
+        <v>985</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="7"/>
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="8"/>
+        <v>1.5000000000000013E-2</v>
+      </c>
+      <c r="I45">
+        <v>5</v>
+      </c>
+      <c r="J45">
+        <v>192</v>
+      </c>
+      <c r="K45">
+        <v>5</v>
+      </c>
+      <c r="L45">
+        <v>5</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="6"/>
+        <v>24.000000000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <f>0.001</f>
+        <v>1E-3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47">
+        <v>108000000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" t="s">
+        <v>6</v>
+      </c>
+      <c r="H49" t="s">
+        <v>8</v>
+      </c>
+      <c r="I49" t="s">
+        <v>19</v>
+      </c>
+      <c r="J49" t="s">
+        <v>20</v>
+      </c>
+      <c r="K49" t="s">
+        <v>21</v>
+      </c>
+      <c r="L49" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>8000</v>
+      </c>
+      <c r="B50">
+        <v>64</v>
+      </c>
+      <c r="C50">
+        <f>B50*A50</f>
+        <v>512000</v>
+      </c>
+      <c r="D50">
+        <v>1000</v>
+      </c>
+      <c r="E50">
+        <v>52</v>
+      </c>
+      <c r="F50" s="1">
+        <f>E50/D50</f>
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="G50" s="1">
+        <f>1-F50</f>
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="I50">
+        <v>4</v>
+      </c>
+      <c r="J50">
+        <v>64</v>
+      </c>
+      <c r="K50">
+        <v>10</v>
+      </c>
+      <c r="L50">
+        <v>25</v>
+      </c>
+      <c r="M50">
+        <f>((1/I50)*J50/(K50*L50))/0.064</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>16000</v>
+      </c>
+      <c r="B51">
+        <v>64</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ref="C51:C73" si="9">B51*A51</f>
+        <v>1024000</v>
+      </c>
+      <c r="D51">
+        <v>1000</v>
+      </c>
+      <c r="E51">
+        <v>108</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" ref="F51:F73" si="10">E51/D51</f>
+        <v>0.108</v>
+      </c>
+      <c r="G51" s="1">
+        <f t="shared" ref="G51:G73" si="11">1-F51</f>
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="I51">
+        <v>4</v>
+      </c>
+      <c r="J51">
+        <v>64</v>
+      </c>
+      <c r="K51">
+        <v>5</v>
+      </c>
+      <c r="L51">
+        <v>25</v>
+      </c>
+      <c r="M51">
+        <f t="shared" ref="M51:M73" si="12">((1/I51)*J51/(K51*L51))/0.064</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>24000</v>
+      </c>
+      <c r="B52">
+        <v>64</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="9"/>
+        <v>1536000</v>
+      </c>
+      <c r="D52">
+        <v>1000</v>
+      </c>
+      <c r="E52">
+        <v>164</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="10"/>
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="G52" s="1">
+        <f t="shared" si="11"/>
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="I52">
+        <v>4</v>
+      </c>
+      <c r="J52">
+        <v>96</v>
+      </c>
+      <c r="K52">
+        <v>5</v>
+      </c>
+      <c r="L52">
+        <v>25</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>32000</v>
+      </c>
+      <c r="B53">
+        <v>64</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="9"/>
+        <v>2048000</v>
+      </c>
+      <c r="D53">
+        <v>1000</v>
+      </c>
+      <c r="E53">
+        <v>212</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="10"/>
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="G53" s="1">
+        <f t="shared" si="11"/>
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="I53">
+        <v>4</v>
+      </c>
+      <c r="J53">
+        <v>128</v>
+      </c>
+      <c r="K53">
+        <v>5</v>
+      </c>
+      <c r="L53">
+        <v>25</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>40000</v>
+      </c>
+      <c r="B54">
+        <v>64</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="9"/>
+        <v>2560000</v>
+      </c>
+      <c r="D54">
+        <v>1000</v>
+      </c>
+      <c r="E54">
+        <v>264</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="10"/>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="G54" s="1">
+        <f t="shared" si="11"/>
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="I54">
+        <v>4</v>
+      </c>
+      <c r="J54">
+        <v>160</v>
+      </c>
+      <c r="K54">
+        <v>5</v>
+      </c>
+      <c r="L54">
+        <v>25</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>48000</v>
+      </c>
+      <c r="B55">
+        <v>64</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="9"/>
+        <v>3072000</v>
+      </c>
+      <c r="D55">
+        <v>1000</v>
+      </c>
+      <c r="E55">
+        <v>316</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="10"/>
+        <v>0.316</v>
+      </c>
+      <c r="G55" s="1">
+        <f t="shared" si="11"/>
+        <v>0.68399999999999994</v>
+      </c>
+      <c r="I55">
+        <v>4</v>
+      </c>
+      <c r="J55">
+        <v>192</v>
+      </c>
+      <c r="K55">
+        <v>5</v>
+      </c>
+      <c r="L55">
+        <v>25</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>56000</v>
+      </c>
+      <c r="B56">
+        <v>64</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="9"/>
+        <v>3584000</v>
+      </c>
+      <c r="D56">
+        <v>1000</v>
+      </c>
+      <c r="E56">
+        <v>372</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="10"/>
+        <v>0.372</v>
+      </c>
+      <c r="G56" s="1">
+        <f t="shared" si="11"/>
+        <v>0.628</v>
+      </c>
+      <c r="I56">
+        <v>5</v>
+      </c>
+      <c r="J56">
+        <v>112</v>
+      </c>
+      <c r="K56">
+        <v>2</v>
+      </c>
+      <c r="L56">
+        <v>25</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="12"/>
+        <v>7.0000000000000009</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>64000</v>
+      </c>
+      <c r="B57">
+        <v>64</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="9"/>
+        <v>4096000</v>
+      </c>
+      <c r="D57">
+        <v>1000</v>
+      </c>
+      <c r="E57">
+        <v>420</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="10"/>
+        <v>0.42</v>
+      </c>
+      <c r="G57" s="1">
+        <f t="shared" si="11"/>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="I57">
+        <v>5</v>
+      </c>
+      <c r="J57">
+        <v>64</v>
+      </c>
+      <c r="K57">
+        <v>5</v>
+      </c>
+      <c r="L57">
+        <v>5</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>72000</v>
+      </c>
+      <c r="B58">
+        <v>64</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="9"/>
+        <v>4608000</v>
+      </c>
+      <c r="D58">
+        <v>1000</v>
+      </c>
+      <c r="E58">
+        <v>476</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="10"/>
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="G58" s="1">
+        <f t="shared" si="11"/>
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="I58">
+        <v>5</v>
+      </c>
+      <c r="J58">
+        <v>72</v>
+      </c>
+      <c r="K58">
+        <v>5</v>
+      </c>
+      <c r="L58">
+        <v>5</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>80000</v>
+      </c>
+      <c r="B59">
+        <v>64</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="9"/>
+        <v>5120000</v>
+      </c>
+      <c r="D59">
+        <v>1000</v>
+      </c>
+      <c r="E59">
+        <v>524</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="10"/>
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="G59" s="1">
+        <f t="shared" si="11"/>
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="I59">
+        <v>5</v>
+      </c>
+      <c r="J59">
+        <v>80</v>
+      </c>
+      <c r="K59">
+        <v>5</v>
+      </c>
+      <c r="L59">
+        <v>5</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>88000</v>
+      </c>
+      <c r="B60">
+        <v>64</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="9"/>
+        <v>5632000</v>
+      </c>
+      <c r="D60">
+        <v>1000</v>
+      </c>
+      <c r="E60">
+        <v>576</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="10"/>
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="G60" s="1">
+        <f t="shared" si="11"/>
+        <v>0.42400000000000004</v>
+      </c>
+      <c r="I60">
+        <v>5</v>
+      </c>
+      <c r="J60">
+        <v>88</v>
+      </c>
+      <c r="K60">
+        <v>5</v>
+      </c>
+      <c r="L60">
+        <v>5</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="12"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>96000</v>
+      </c>
+      <c r="B61">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="9"/>
+        <v>6144000</v>
+      </c>
+      <c r="D61">
+        <v>1000</v>
+      </c>
+      <c r="E61">
+        <v>628</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="10"/>
+        <v>0.628</v>
+      </c>
+      <c r="G61" s="1">
+        <f t="shared" si="11"/>
+        <v>0.372</v>
+      </c>
+      <c r="I61">
+        <v>5</v>
+      </c>
+      <c r="J61">
+        <v>96</v>
+      </c>
+      <c r="K61">
+        <v>5</v>
+      </c>
+      <c r="L61">
+        <v>5</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="12"/>
+        <v>12.000000000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>104000</v>
+      </c>
+      <c r="B62">
+        <v>64</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="9"/>
+        <v>6656000</v>
+      </c>
+      <c r="D62">
+        <v>1000</v>
+      </c>
+      <c r="E62">
+        <v>680</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="10"/>
+        <v>0.68</v>
+      </c>
+      <c r="G62" s="1">
+        <f t="shared" si="11"/>
+        <v>0.31999999999999995</v>
+      </c>
+      <c r="I62">
+        <v>5</v>
+      </c>
+      <c r="J62">
+        <v>104</v>
+      </c>
+      <c r="K62">
+        <v>5</v>
+      </c>
+      <c r="L62">
+        <v>5</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="12"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>112000</v>
+      </c>
+      <c r="B63">
+        <v>64</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="9"/>
+        <v>7168000</v>
+      </c>
+      <c r="D63">
+        <v>1000</v>
+      </c>
+      <c r="E63">
+        <v>732</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="10"/>
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="G63" s="1">
+        <f t="shared" si="11"/>
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="I63">
+        <v>5</v>
+      </c>
+      <c r="J63">
+        <v>112</v>
+      </c>
+      <c r="K63">
+        <v>5</v>
+      </c>
+      <c r="L63">
+        <v>5</v>
+      </c>
+      <c r="M63">
+        <f t="shared" si="12"/>
+        <v>14.000000000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>120000</v>
+      </c>
+      <c r="B64">
+        <v>64</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="9"/>
+        <v>7680000</v>
+      </c>
+      <c r="D64">
+        <v>1000</v>
+      </c>
+      <c r="E64">
+        <v>784</v>
+      </c>
+      <c r="F64" s="1">
+        <f t="shared" si="10"/>
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="G64" s="1">
+        <f t="shared" si="11"/>
+        <v>0.21599999999999997</v>
+      </c>
+      <c r="I64">
+        <v>5</v>
+      </c>
+      <c r="J64">
+        <v>120</v>
+      </c>
+      <c r="K64">
+        <v>5</v>
+      </c>
+      <c r="L64">
+        <v>5</v>
+      </c>
+      <c r="M64">
+        <f t="shared" si="12"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>128000</v>
+      </c>
+      <c r="B65">
+        <v>64</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="9"/>
+        <v>8192000</v>
+      </c>
+      <c r="D65">
+        <v>1000</v>
+      </c>
+      <c r="E65">
+        <v>840</v>
+      </c>
+      <c r="F65" s="1">
+        <f t="shared" si="10"/>
+        <v>0.84</v>
+      </c>
+      <c r="G65" s="1">
+        <f t="shared" si="11"/>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="I65">
+        <v>5</v>
+      </c>
+      <c r="J65">
+        <v>128</v>
+      </c>
+      <c r="K65">
+        <v>5</v>
+      </c>
+      <c r="L65">
+        <v>5</v>
+      </c>
+      <c r="M65">
+        <f t="shared" si="12"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>136000</v>
+      </c>
+      <c r="B66">
+        <v>64</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="9"/>
+        <v>8704000</v>
+      </c>
+      <c r="D66">
+        <v>1000</v>
+      </c>
+      <c r="E66">
+        <v>892</v>
+      </c>
+      <c r="F66" s="1">
+        <f t="shared" si="10"/>
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="G66" s="1">
+        <f t="shared" si="11"/>
+        <v>0.10799999999999998</v>
+      </c>
+      <c r="I66">
+        <v>5</v>
+      </c>
+      <c r="J66">
+        <v>136</v>
+      </c>
+      <c r="K66">
+        <v>5</v>
+      </c>
+      <c r="L66">
+        <v>5</v>
+      </c>
+      <c r="M66">
+        <f t="shared" si="12"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>144000</v>
+      </c>
+      <c r="B67">
+        <v>64</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="9"/>
+        <v>9216000</v>
+      </c>
+      <c r="D67">
+        <v>1000</v>
+      </c>
+      <c r="E67">
+        <v>940</v>
+      </c>
+      <c r="F67" s="1">
+        <f t="shared" si="10"/>
+        <v>0.94</v>
+      </c>
+      <c r="G67" s="1">
+        <f t="shared" si="11"/>
+        <v>6.0000000000000053E-2</v>
+      </c>
+      <c r="I67">
+        <v>5</v>
+      </c>
+      <c r="J67">
+        <v>144</v>
+      </c>
+      <c r="K67">
+        <v>5</v>
+      </c>
+      <c r="L67">
+        <v>5</v>
+      </c>
+      <c r="M67">
+        <f t="shared" si="12"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>152000</v>
+      </c>
+      <c r="B68">
+        <v>64</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="9"/>
+        <v>9728000</v>
+      </c>
+      <c r="D68">
+        <v>1000</v>
+      </c>
+      <c r="E68">
+        <v>995</v>
+      </c>
+      <c r="F68" s="1">
+        <f t="shared" si="10"/>
+        <v>0.995</v>
+      </c>
+      <c r="G68" s="1">
+        <f t="shared" si="11"/>
+        <v>5.0000000000000044E-3</v>
+      </c>
+      <c r="I68">
+        <v>5</v>
+      </c>
+      <c r="J68">
+        <v>152</v>
+      </c>
+      <c r="K68">
+        <v>5</v>
+      </c>
+      <c r="L68">
+        <v>5</v>
+      </c>
+      <c r="M68">
+        <f t="shared" si="12"/>
+        <v>19.000000000000004</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>160000</v>
+      </c>
+      <c r="B69">
+        <v>64</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="9"/>
+        <v>10240000</v>
+      </c>
+      <c r="D69">
+        <v>1000</v>
+      </c>
+      <c r="E69">
+        <v>1060</v>
+      </c>
+      <c r="F69" s="1">
+        <f t="shared" si="10"/>
+        <v>1.06</v>
+      </c>
+      <c r="G69" s="1">
+        <f t="shared" si="11"/>
+        <v>-6.0000000000000053E-2</v>
+      </c>
+      <c r="I69">
+        <v>5</v>
+      </c>
+      <c r="J69">
+        <v>160</v>
+      </c>
+      <c r="K69">
+        <v>5</v>
+      </c>
+      <c r="L69">
+        <v>5</v>
+      </c>
+      <c r="M69">
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>168000</v>
+      </c>
+      <c r="B70">
+        <v>64</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="9"/>
+        <v>10752000</v>
+      </c>
+      <c r="D70">
+        <v>1000</v>
+      </c>
+      <c r="F70" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="G70" s="1">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>5</v>
+      </c>
+      <c r="J70">
+        <v>168</v>
+      </c>
+      <c r="K70">
+        <v>5</v>
+      </c>
+      <c r="L70">
+        <v>5</v>
+      </c>
+      <c r="M70">
+        <f t="shared" si="12"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>176000</v>
+      </c>
+      <c r="B71">
+        <v>64</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="9"/>
+        <v>11264000</v>
+      </c>
+      <c r="D71">
+        <v>1000</v>
+      </c>
+      <c r="F71" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="G71" s="1">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>5</v>
+      </c>
+      <c r="J71">
+        <v>176</v>
+      </c>
+      <c r="K71">
+        <v>5</v>
+      </c>
+      <c r="L71">
+        <v>5</v>
+      </c>
+      <c r="M71">
+        <f t="shared" si="12"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>184000</v>
+      </c>
+      <c r="B72">
+        <v>64</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="9"/>
+        <v>11776000</v>
+      </c>
+      <c r="D72">
+        <v>1000</v>
+      </c>
+      <c r="F72" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="G72" s="1">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>5</v>
+      </c>
+      <c r="J72">
+        <v>184</v>
+      </c>
+      <c r="K72">
+        <v>5</v>
+      </c>
+      <c r="L72">
+        <v>5</v>
+      </c>
+      <c r="M72">
+        <f t="shared" si="12"/>
+        <v>23.000000000000004</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>192000</v>
+      </c>
+      <c r="B73">
+        <v>64</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="9"/>
+        <v>12288000</v>
+      </c>
+      <c r="D73">
+        <v>1000</v>
+      </c>
+      <c r="F73" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="G73" s="1">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <v>5</v>
+      </c>
+      <c r="J73">
+        <v>192</v>
+      </c>
+      <c r="K73">
+        <v>5</v>
+      </c>
+      <c r="L73">
+        <v>5</v>
+      </c>
+      <c r="M73">
+        <f t="shared" si="12"/>
+        <v>24.000000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>